<commit_message>
Adding Paramters & adding data to Queue
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -151,9 +151,6 @@
     <t>System exception.</t>
   </si>
   <si>
-    <t>demoProcessQueue</t>
-  </si>
-  <si>
     <t>ProjectId</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>IsupplierDevUserid</t>
+  </si>
+  <si>
+    <t>MassUploadData</t>
   </si>
 </sst>
 </file>
@@ -598,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,18 +625,18 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -677,49 +677,49 @@
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -901,24 +901,24 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
         <v>47</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>53</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
@@ -971,18 +971,18 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>